<commit_message>
Added some stuff to EDA
</commit_message>
<xml_diff>
--- a/AI Assignment - Tasks.xlsx
+++ b/AI Assignment - Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icthva-my.sharepoint.com/personal/jp_britten_hva_nl/Documents/HvA/Digital Driven Business Masters/AI Methods for Business/Assignment Files/DDB_AI_Group_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65C4388D-1D96-8E47-9AB2-151B276710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{65C4388D-1D96-8E47-9AB2-151B276710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45F7254-FCD3-B447-9270-C0C813E11A30}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="680" windowWidth="27080" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
   <si>
     <r>
       <rPr>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>Cleanup, markdown, visuals.</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1246,7 +1249,9 @@
       <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="F8" s="10" t="s">
         <v>26</v>
       </c>
@@ -1827,8 +1832,12 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="E33" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G33" s="7" t="s">
         <v>80</v>
       </c>
@@ -1846,8 +1855,12 @@
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
+      <c r="E34" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G34" s="7" t="s">
         <v>82</v>
       </c>
@@ -1865,8 +1878,12 @@
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
+      <c r="E35" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G35" s="7" t="s">
         <v>84</v>
       </c>
@@ -1884,8 +1901,12 @@
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
+      <c r="E36" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G36" s="7" t="s">
         <v>86</v>
       </c>
@@ -1903,8 +1924,12 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
+      <c r="E37" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G37" s="7" t="s">
         <v>88</v>
       </c>
@@ -2209,8 +2234,12 @@
       <c r="D53" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="10"/>
+      <c r="E53" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G53" s="7" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
Added my name into some tasks
</commit_message>
<xml_diff>
--- a/AI Assignment - Tasks.xlsx
+++ b/AI Assignment - Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icthva-my.sharepoint.com/personal/jp_britten_hva_nl/Documents/HvA/Digital Driven Business Masters/AI Methods for Business/Assignment Files/DDB_AI_Group_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{65C4388D-1D96-8E47-9AB2-151B276710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45F7254-FCD3-B447-9270-C0C813E11A30}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{65C4388D-1D96-8E47-9AB2-151B276710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C67C6FF5-91BF-8A49-B488-898B9611AB2A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="680" windowWidth="27080" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="126">
   <si>
     <r>
       <rPr>
@@ -498,6 +498,9 @@
   <si>
     <t>Not Started</t>
   </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
 </sst>
 </file>
 
@@ -506,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +549,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -686,7 +695,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1059,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1179,9 @@
       <c r="D3" s="8">
         <v>45700</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="F3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1204,9 @@
       <c r="D4" s="8">
         <v>45700</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="F4" s="10" t="s">
         <v>12</v>
       </c>
@@ -1176,7 +1229,9 @@
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
@@ -2274,6 +2329,7 @@
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="F12:F27"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F3:F51 F53:F54">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"All"</formula>

</xml_diff>